<commit_message>
adding files missed by mistake
</commit_message>
<xml_diff>
--- a/Assignment3/dataset/en_conditions.xlsx
+++ b/Assignment3/dataset/en_conditions.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="162">
   <si>
     <t xml:space="preserve">word1</t>
   </si>
@@ -355,48 +355,6 @@
     <t xml:space="preserve">berid</t>
   </si>
   <si>
-    <t xml:space="preserve">entehvain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bryccyli</t>
-  </si>
-  <si>
-    <t xml:space="preserve">angeatec</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hodker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">suem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">builde</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rigaen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wuncir</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dvsagceeieni</t>
-  </si>
-  <si>
-    <t xml:space="preserve">turpit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">crlceet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chulk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">incuire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gway</t>
-  </si>
-  <si>
     <t xml:space="preserve">invent</t>
   </si>
   <si>
@@ -472,48 +430,6 @@
     <t xml:space="preserve">bygknner</t>
   </si>
   <si>
-    <t xml:space="preserve">separate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bext</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">blumi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cents</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rankep</t>
-  </si>
-  <si>
-    <t xml:space="preserve">finished</t>
-  </si>
-  <si>
-    <t xml:space="preserve">blxw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pastry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">weue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">heroine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">losh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">confuse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">crtuain</t>
-  </si>
-  <si>
     <t xml:space="preserve">riject</t>
   </si>
   <si>
@@ -590,42 +506,6 @@
   </si>
   <si>
     <t xml:space="preserve">fashion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sastir</t>
-  </si>
-  <si>
-    <t xml:space="preserve">failure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rntractr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tomer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">elephant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">blaokbonvd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">disagree</t>
-  </si>
-  <si>
-    <t xml:space="preserve">povtecy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ktcheken</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cotton</t>
   </si>
 </sst>
 </file>
@@ -640,6 +520,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -660,6 +541,7 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -730,10 +612,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:D81"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A76" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B99" activeCellId="0" sqref="B99"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D68" activeCellId="0" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1508,7 +1390,7 @@
         <v>86</v>
       </c>
       <c r="D55" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1522,7 +1404,7 @@
         <v>86</v>
       </c>
       <c r="D56" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1536,7 +1418,7 @@
         <v>86</v>
       </c>
       <c r="D57" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1550,7 +1432,7 @@
         <v>86</v>
       </c>
       <c r="D58" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1564,7 +1446,7 @@
         <v>86</v>
       </c>
       <c r="D59" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1578,7 +1460,7 @@
         <v>86</v>
       </c>
       <c r="D60" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1592,15 +1474,15 @@
         <v>86</v>
       </c>
       <c r="D61" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>86</v>
@@ -1611,10 +1493,10 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>128</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>86</v>
@@ -1625,10 +1507,10 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>130</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>86</v>
@@ -1639,10 +1521,10 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>86</v>
@@ -1653,10 +1535,10 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B66" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>86</v>
@@ -1667,10 +1549,10 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>136</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>86</v>
@@ -1681,21 +1563,21 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>138</v>
-      </c>
       <c r="C68" s="1" t="s">
         <v>86</v>
       </c>
       <c r="D68" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>57</v>
+        <v>138</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>139</v>
@@ -1704,7 +1586,7 @@
         <v>86</v>
       </c>
       <c r="D69" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1718,7 +1600,7 @@
         <v>86</v>
       </c>
       <c r="D70" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1732,7 +1614,7 @@
         <v>86</v>
       </c>
       <c r="D71" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1746,7 +1628,7 @@
         <v>86</v>
       </c>
       <c r="D72" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1760,7 +1642,7 @@
         <v>86</v>
       </c>
       <c r="D73" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1768,390 +1650,110 @@
         <v>148</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>149</v>
+        <v>73</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>86</v>
       </c>
       <c r="D74" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B75" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B75" s="1" t="s">
-        <v>151</v>
-      </c>
       <c r="C75" s="1" t="s">
         <v>86</v>
       </c>
       <c r="D75" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B76" s="1" t="s">
-        <v>153</v>
-      </c>
       <c r="C76" s="1" t="s">
         <v>86</v>
       </c>
       <c r="D76" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B77" s="1" t="s">
-        <v>155</v>
-      </c>
       <c r="C77" s="1" t="s">
         <v>86</v>
       </c>
       <c r="D77" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B78" s="1" t="s">
-        <v>157</v>
-      </c>
       <c r="C78" s="1" t="s">
         <v>86</v>
       </c>
       <c r="D78" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B79" s="1" t="s">
-        <v>159</v>
-      </c>
       <c r="C79" s="1" t="s">
         <v>86</v>
       </c>
       <c r="D79" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>161</v>
+        <v>130</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>86</v>
       </c>
       <c r="D80" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>86</v>
       </c>
       <c r="D81" s="1" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D82" s="1" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D83" s="1" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D84" s="1" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D85" s="1" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D86" s="1" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D87" s="1" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D88" s="1" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D89" s="1" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D90" s="1" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D91" s="1" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D92" s="1" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D93" s="1" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D94" s="1" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D95" s="1" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D96" s="1" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D97" s="1" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D98" s="1" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D99" s="1" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D100" s="1" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D101" s="1" t="n">
         <v>4</v>
       </c>
     </row>

</xml_diff>